<commit_message>
final update of Dataset S1
</commit_message>
<xml_diff>
--- a/Dataset.S1.xlsx
+++ b/Dataset.S1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DanielPaluh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DanielPaluh/Documents/Projects/published/hyperossification/ACCEPTED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BDFE1B-2E79-4643-8BD7-DA0D4EFDB9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7CA5FA-C868-4344-9230-9DABD0BCE4AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23420" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classifier" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="562">
   <si>
     <t>Family</t>
   </si>
@@ -1706,6 +1706,9 @@
   </si>
   <si>
     <t>amnh:herpetology:a-41823</t>
+  </si>
+  <si>
+    <t>doi:10.17602/M2/M50228</t>
   </si>
 </sst>
 </file>
@@ -2636,7 +2639,7 @@
   <dimension ref="A1:N161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8893,7 +8896,7 @@
         <v>335</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>540</v>
+        <v>561</v>
       </c>
       <c r="L142" s="8" t="s">
         <v>390</v>
@@ -9787,43 +9790,44 @@
     <hyperlink ref="K139" r:id="rId119" display="https://doi.org/10.17602/M2/M11082" xr:uid="{55F0BE28-D3A5-F045-B7EC-AB8F2B5A3CEC}"/>
     <hyperlink ref="K140" r:id="rId120" display="https://doi.org/10.17602/M2/M37817" xr:uid="{1923E0F8-3462-1948-A17E-C981AF047C4E}"/>
     <hyperlink ref="K141" r:id="rId121" display="https://doi.org/10.17602/M2/M24024" xr:uid="{49290E01-B7D3-3542-817F-0C4259016692}"/>
-    <hyperlink ref="K142" r:id="rId122" display="https://doi.org/10.17602/M2/M24024" xr:uid="{C0996689-D996-6240-9DD8-DAAD8FD1B125}"/>
-    <hyperlink ref="K143" r:id="rId123" display="https://doi.org/10.17602/M2/M84514" xr:uid="{4131332A-0A79-8741-B3EC-CFC6C0E1B2EF}"/>
-    <hyperlink ref="K144" r:id="rId124" display="https://doi.org/10.17602/M2/M24426" xr:uid="{D692578F-C263-F441-AE06-6FC1F2C597A8}"/>
-    <hyperlink ref="K145" r:id="rId125" display="https://doi.org/10.17602/M2/M20347" xr:uid="{C4515EE0-3306-124C-90D6-BFA8D0D99B45}"/>
-    <hyperlink ref="K146" r:id="rId126" display="https://doi.org/10.17602/M2/M42671" xr:uid="{8B56FB89-CFDD-8444-AE80-355A23427B61}"/>
-    <hyperlink ref="K147" r:id="rId127" display="https://doi.org/10.17602/M2/M37692" xr:uid="{EA8EE419-1EF1-C64A-8564-C672A45D1650}"/>
-    <hyperlink ref="K148" r:id="rId128" display="https://doi.org/10.17602/M2/M50092" xr:uid="{2B857FCE-E505-6F40-95C3-27AEE6684927}"/>
-    <hyperlink ref="K149" r:id="rId129" display="https://doi.org/10.17602/M2/M24448" xr:uid="{B29C2258-2BF0-DE45-A50B-7E25B991B2CC}"/>
-    <hyperlink ref="K151" r:id="rId130" display="https://doi.org/10.17602/M2/M25656" xr:uid="{F3EC92E4-CC15-6B4E-AED7-AF9116AFB02D}"/>
-    <hyperlink ref="K153" r:id="rId131" display="https://doi.org/10.17602/M2/M27178" xr:uid="{5D3B224F-8EF0-514C-9CA0-2888647AE7E9}"/>
-    <hyperlink ref="K154" r:id="rId132" display="https://doi.org/10.17602/M2/M49261" xr:uid="{31BB0ACA-A0D4-3048-AA20-351C34EF78A7}"/>
-    <hyperlink ref="K156" r:id="rId133" display="https://doi.org/10.17602/M2/M34354" xr:uid="{32B8170F-7527-C048-825F-A2553582BA4B}"/>
-    <hyperlink ref="K158" r:id="rId134" display="https://doi.org/10.17602/M2/M38057" xr:uid="{701FB912-7C26-484B-A2CA-03D259D3E7C6}"/>
-    <hyperlink ref="K159" r:id="rId135" display="https://doi.org/10.17602/M2/M49919" xr:uid="{AF93CDC9-402F-594E-888E-2D601A4729E2}"/>
-    <hyperlink ref="K55" r:id="rId136" display="https://doi.org/10.17602/M2/M101101" xr:uid="{449C7806-566C-1B43-A7AE-3D9522C49FF2}"/>
-    <hyperlink ref="K76" r:id="rId137" display="https://doi.org/10.17602/M2/M22195" xr:uid="{62BE8B52-6239-1148-AB77-7C32FCBD5AD1}"/>
-    <hyperlink ref="K70" r:id="rId138" display="https://doi.org/10.17602/M2/M101128" xr:uid="{1D6B44CD-8F72-5A4A-9185-C4047CD39A2D}"/>
-    <hyperlink ref="K157" r:id="rId139" display="https://doi.org/10.17602/M2/M101167" xr:uid="{2A8A151F-F170-A641-B63C-4B559F98F10D}"/>
-    <hyperlink ref="K155" r:id="rId140" display="https://doi.org/10.17602/M2/M101177" xr:uid="{36F06B4A-A43F-5644-A2DF-03C36FECD225}"/>
-    <hyperlink ref="K152" r:id="rId141" display="https://doi.org/10.17602/M2/M101183" xr:uid="{E4FF972E-712D-0B48-9535-D1F7C0AC1A51}"/>
-    <hyperlink ref="K150" r:id="rId142" display="https://doi.org/10.17602/M2/M101185" xr:uid="{276EE588-AA66-AC43-B147-FA79B75DDFCB}"/>
-    <hyperlink ref="K137" r:id="rId143" display="https://doi.org/10.17602/M2/M101187" xr:uid="{5B4FB4C2-D103-244E-929D-7FC731F82E40}"/>
-    <hyperlink ref="K129" r:id="rId144" display="https://doi.org/10.17602/M2/M48893" xr:uid="{96B0A88E-D559-AA46-9150-16E06A35AECC}"/>
-    <hyperlink ref="K136" r:id="rId145" display="https://doi.org/10.17602/M2/M101188" xr:uid="{A4C8DD5C-49DF-714B-B9DE-36C6FC542303}"/>
-    <hyperlink ref="K124" r:id="rId146" display="https://doi.org/10.17602/M2/M101191" xr:uid="{A4FD34E6-BC68-7543-A560-0A773C4C8B2F}"/>
-    <hyperlink ref="K105" r:id="rId147" display="https://doi.org/10.17602/M2/M49377" xr:uid="{7BD409D6-CEC2-B048-8192-4DFF23F0BD19}"/>
-    <hyperlink ref="K104" r:id="rId148" xr:uid="{F2508140-1E51-5444-B664-D1E01B3108E8}"/>
-    <hyperlink ref="K101" r:id="rId149" display="https://doi.org/10.17602/M2/M34831" xr:uid="{B7519FF5-A8BA-6D4B-8FCD-90FD47E1C6FD}"/>
-    <hyperlink ref="K88" r:id="rId150" display="https://doi.org/10.17602/M2/M49968" xr:uid="{E507CDC2-090B-594E-B44A-21422F71080A}"/>
-    <hyperlink ref="K84" r:id="rId151" display="https://doi.org/10.17602/M2/M55512" xr:uid="{440A78DA-B71E-B540-9AA4-2219250ECF13}"/>
-    <hyperlink ref="K120" r:id="rId152" display="https://doi.org/10.17602/M2/M101192" xr:uid="{55FDF681-3FEF-F641-8DE9-85D04B41489F}"/>
-    <hyperlink ref="K97" r:id="rId153" display="https://doi.org/10.17602/M2/M49385" xr:uid="{CED78F49-DE70-A54F-95C6-E474E69FB400}"/>
-    <hyperlink ref="K117" r:id="rId154" display="https://doi.org/10.17602/M2/M101194" xr:uid="{3D91F4C0-17BC-854D-BFC8-89B1DA13171C}"/>
-    <hyperlink ref="K102" r:id="rId155" display="https://doi.org/10.17602/M2/M101195" xr:uid="{1EC0744B-4442-0D48-A6F2-00A6C0BD7A21}"/>
-    <hyperlink ref="K100" r:id="rId156" display="https://doi.org/10.17602/M2/M101196" xr:uid="{90618EBE-DE7E-6D47-83E3-4E41429A53F9}"/>
-    <hyperlink ref="K77" r:id="rId157" display="https://doi.org/10.17602/M2/M101179" xr:uid="{ADC70FD0-D92E-DD43-97EC-7FF8D21C739F}"/>
+    <hyperlink ref="K143" r:id="rId122" display="https://doi.org/10.17602/M2/M84514" xr:uid="{4131332A-0A79-8741-B3EC-CFC6C0E1B2EF}"/>
+    <hyperlink ref="K144" r:id="rId123" display="https://doi.org/10.17602/M2/M24426" xr:uid="{D692578F-C263-F441-AE06-6FC1F2C597A8}"/>
+    <hyperlink ref="K145" r:id="rId124" display="https://doi.org/10.17602/M2/M20347" xr:uid="{C4515EE0-3306-124C-90D6-BFA8D0D99B45}"/>
+    <hyperlink ref="K146" r:id="rId125" display="https://doi.org/10.17602/M2/M42671" xr:uid="{8B56FB89-CFDD-8444-AE80-355A23427B61}"/>
+    <hyperlink ref="K147" r:id="rId126" display="https://doi.org/10.17602/M2/M37692" xr:uid="{EA8EE419-1EF1-C64A-8564-C672A45D1650}"/>
+    <hyperlink ref="K148" r:id="rId127" display="https://doi.org/10.17602/M2/M50092" xr:uid="{2B857FCE-E505-6F40-95C3-27AEE6684927}"/>
+    <hyperlink ref="K149" r:id="rId128" display="https://doi.org/10.17602/M2/M24448" xr:uid="{B29C2258-2BF0-DE45-A50B-7E25B991B2CC}"/>
+    <hyperlink ref="K151" r:id="rId129" display="https://doi.org/10.17602/M2/M25656" xr:uid="{F3EC92E4-CC15-6B4E-AED7-AF9116AFB02D}"/>
+    <hyperlink ref="K153" r:id="rId130" display="https://doi.org/10.17602/M2/M27178" xr:uid="{5D3B224F-8EF0-514C-9CA0-2888647AE7E9}"/>
+    <hyperlink ref="K154" r:id="rId131" display="https://doi.org/10.17602/M2/M49261" xr:uid="{31BB0ACA-A0D4-3048-AA20-351C34EF78A7}"/>
+    <hyperlink ref="K156" r:id="rId132" display="https://doi.org/10.17602/M2/M34354" xr:uid="{32B8170F-7527-C048-825F-A2553582BA4B}"/>
+    <hyperlink ref="K158" r:id="rId133" display="https://doi.org/10.17602/M2/M38057" xr:uid="{701FB912-7C26-484B-A2CA-03D259D3E7C6}"/>
+    <hyperlink ref="K159" r:id="rId134" display="https://doi.org/10.17602/M2/M49919" xr:uid="{AF93CDC9-402F-594E-888E-2D601A4729E2}"/>
+    <hyperlink ref="K55" r:id="rId135" display="https://doi.org/10.17602/M2/M101101" xr:uid="{449C7806-566C-1B43-A7AE-3D9522C49FF2}"/>
+    <hyperlink ref="K76" r:id="rId136" display="https://doi.org/10.17602/M2/M22195" xr:uid="{62BE8B52-6239-1148-AB77-7C32FCBD5AD1}"/>
+    <hyperlink ref="K70" r:id="rId137" display="https://doi.org/10.17602/M2/M101128" xr:uid="{1D6B44CD-8F72-5A4A-9185-C4047CD39A2D}"/>
+    <hyperlink ref="K157" r:id="rId138" display="https://doi.org/10.17602/M2/M101167" xr:uid="{2A8A151F-F170-A641-B63C-4B559F98F10D}"/>
+    <hyperlink ref="K155" r:id="rId139" display="https://doi.org/10.17602/M2/M101177" xr:uid="{36F06B4A-A43F-5644-A2DF-03C36FECD225}"/>
+    <hyperlink ref="K152" r:id="rId140" display="https://doi.org/10.17602/M2/M101183" xr:uid="{E4FF972E-712D-0B48-9535-D1F7C0AC1A51}"/>
+    <hyperlink ref="K150" r:id="rId141" display="https://doi.org/10.17602/M2/M101185" xr:uid="{276EE588-AA66-AC43-B147-FA79B75DDFCB}"/>
+    <hyperlink ref="K137" r:id="rId142" display="https://doi.org/10.17602/M2/M101187" xr:uid="{5B4FB4C2-D103-244E-929D-7FC731F82E40}"/>
+    <hyperlink ref="K129" r:id="rId143" display="https://doi.org/10.17602/M2/M48893" xr:uid="{96B0A88E-D559-AA46-9150-16E06A35AECC}"/>
+    <hyperlink ref="K136" r:id="rId144" display="https://doi.org/10.17602/M2/M101188" xr:uid="{A4C8DD5C-49DF-714B-B9DE-36C6FC542303}"/>
+    <hyperlink ref="K124" r:id="rId145" display="https://doi.org/10.17602/M2/M101191" xr:uid="{A4FD34E6-BC68-7543-A560-0A773C4C8B2F}"/>
+    <hyperlink ref="K105" r:id="rId146" display="https://doi.org/10.17602/M2/M49377" xr:uid="{7BD409D6-CEC2-B048-8192-4DFF23F0BD19}"/>
+    <hyperlink ref="K104" r:id="rId147" xr:uid="{F2508140-1E51-5444-B664-D1E01B3108E8}"/>
+    <hyperlink ref="K101" r:id="rId148" display="https://doi.org/10.17602/M2/M34831" xr:uid="{B7519FF5-A8BA-6D4B-8FCD-90FD47E1C6FD}"/>
+    <hyperlink ref="K88" r:id="rId149" display="https://doi.org/10.17602/M2/M49968" xr:uid="{E507CDC2-090B-594E-B44A-21422F71080A}"/>
+    <hyperlink ref="K84" r:id="rId150" display="https://doi.org/10.17602/M2/M55512" xr:uid="{440A78DA-B71E-B540-9AA4-2219250ECF13}"/>
+    <hyperlink ref="K120" r:id="rId151" display="https://doi.org/10.17602/M2/M101192" xr:uid="{55FDF681-3FEF-F641-8DE9-85D04B41489F}"/>
+    <hyperlink ref="K97" r:id="rId152" display="https://doi.org/10.17602/M2/M49385" xr:uid="{CED78F49-DE70-A54F-95C6-E474E69FB400}"/>
+    <hyperlink ref="K117" r:id="rId153" display="https://doi.org/10.17602/M2/M101194" xr:uid="{3D91F4C0-17BC-854D-BFC8-89B1DA13171C}"/>
+    <hyperlink ref="K102" r:id="rId154" display="https://doi.org/10.17602/M2/M101195" xr:uid="{1EC0744B-4442-0D48-A6F2-00A6C0BD7A21}"/>
+    <hyperlink ref="K100" r:id="rId155" display="https://doi.org/10.17602/M2/M101196" xr:uid="{90618EBE-DE7E-6D47-83E3-4E41429A53F9}"/>
+    <hyperlink ref="K77" r:id="rId156" display="https://doi.org/10.17602/M2/M101179" xr:uid="{ADC70FD0-D92E-DD43-97EC-7FF8D21C739F}"/>
+    <hyperlink ref="K142" r:id="rId157" display="https://doi.org/10.17602/M2/M50228" xr:uid="{710FA44A-2875-7540-9613-86EDE41C0BE1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>